<commit_message>
added a notes section
</commit_message>
<xml_diff>
--- a/2016summerWeeklyReports/RoboLabTimesheet.xlsx
+++ b/2016summerWeeklyReports/RoboLabTimesheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="-1000" yWindow="440" windowWidth="25360" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>2016.05.18</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Name:</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>e.g.:  On Monday I worked at the testing site and was not in the lab</t>
   </si>
 </sst>
 </file>
@@ -244,7 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -254,14 +260,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -594,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X25"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -625,12 +632,12 @@
     <col min="23" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:26">
       <c r="B1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:26">
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -653,186 +660,192 @@
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
     </row>
-    <row r="3" spans="1:24">
-      <c r="C3" s="7" t="s">
+    <row r="3" spans="1:26">
+      <c r="C3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7" t="s">
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7" t="s">
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7" t="s">
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7" t="s">
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7" t="s">
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
       <c r="X3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="Z3" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="1"/>
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="O4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="P4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="Q4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="R4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="S4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="T4" s="11" t="s">
+      <c r="T4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="U4" s="9" t="s">
+      <c r="U4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="V4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="W4" s="11" t="s">
+      <c r="W4" s="10" t="s">
         <v>24</v>
       </c>
       <c r="X4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="Z4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="12">
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11">
         <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" s="8">
-        <v>0</v>
-      </c>
-      <c r="I5" s="12">
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11">
         <v>0</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
-      <c r="K5" s="8">
-        <v>0</v>
-      </c>
-      <c r="L5" s="12">
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11">
         <v>0</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="N5" s="8">
-        <v>0</v>
-      </c>
-      <c r="O5" s="12">
+      <c r="N5" s="7">
+        <v>0</v>
+      </c>
+      <c r="O5" s="11">
         <v>0</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
-      <c r="Q5" s="8">
-        <v>0</v>
-      </c>
-      <c r="R5" s="12">
+      <c r="Q5" s="7">
+        <v>0</v>
+      </c>
+      <c r="R5" s="11">
         <v>0</v>
       </c>
       <c r="S5">
         <v>0</v>
       </c>
-      <c r="T5" s="8">
-        <v>0</v>
-      </c>
-      <c r="U5" s="12">
+      <c r="T5" s="7">
+        <v>0</v>
+      </c>
+      <c r="U5" s="11">
         <v>0</v>
       </c>
       <c r="V5">
         <v>0</v>
       </c>
-      <c r="W5" s="8">
+      <c r="W5" s="7">
         <v>0</v>
       </c>
       <c r="X5">
@@ -840,74 +853,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:26">
       <c r="A6" s="2">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11">
         <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6" s="8">
-        <v>0</v>
-      </c>
-      <c r="I6" s="12">
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="11">
         <v>0</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
-      <c r="K6" s="8">
-        <v>0</v>
-      </c>
-      <c r="L6" s="12">
+      <c r="K6" s="7">
+        <v>0</v>
+      </c>
+      <c r="L6" s="11">
         <v>0</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6" s="8">
-        <v>0</v>
-      </c>
-      <c r="O6" s="12">
+      <c r="N6" s="7">
+        <v>0</v>
+      </c>
+      <c r="O6" s="11">
         <v>0</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
-      <c r="Q6" s="8">
-        <v>0</v>
-      </c>
-      <c r="R6" s="12">
+      <c r="Q6" s="7">
+        <v>0</v>
+      </c>
+      <c r="R6" s="11">
         <v>0</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
-      <c r="T6" s="8">
-        <v>0</v>
-      </c>
-      <c r="U6" s="12">
+      <c r="T6" s="7">
+        <v>0</v>
+      </c>
+      <c r="U6" s="11">
         <v>0</v>
       </c>
       <c r="V6">
         <v>0</v>
       </c>
-      <c r="W6" s="8">
+      <c r="W6" s="7">
         <v>0</v>
       </c>
       <c r="X6">
@@ -915,74 +928,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:26">
       <c r="A7" s="2">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="12">
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11">
         <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
-      <c r="I7" s="12">
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11">
         <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
-      <c r="K7" s="8">
-        <v>0</v>
-      </c>
-      <c r="L7" s="12">
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11">
         <v>0</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7" s="8">
-        <v>0</v>
-      </c>
-      <c r="O7" s="12">
+      <c r="N7" s="7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="11">
         <v>0</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
-      <c r="Q7" s="8">
-        <v>0</v>
-      </c>
-      <c r="R7" s="12">
+      <c r="Q7" s="7">
+        <v>0</v>
+      </c>
+      <c r="R7" s="11">
         <v>0</v>
       </c>
       <c r="S7">
         <v>0</v>
       </c>
-      <c r="T7" s="8">
-        <v>0</v>
-      </c>
-      <c r="U7" s="12">
+      <c r="T7" s="7">
+        <v>0</v>
+      </c>
+      <c r="U7" s="11">
         <v>0</v>
       </c>
       <c r="V7">
         <v>0</v>
       </c>
-      <c r="W7" s="8">
+      <c r="W7" s="7">
         <v>0</v>
       </c>
       <c r="X7">
@@ -990,74 +1003,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:26">
       <c r="A8" s="2">
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="12">
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11">
         <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8" s="8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="12">
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
         <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
-      <c r="K8" s="8">
-        <v>0</v>
-      </c>
-      <c r="L8" s="12">
+      <c r="K8" s="7">
+        <v>0</v>
+      </c>
+      <c r="L8" s="11">
         <v>0</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8" s="8">
-        <v>0</v>
-      </c>
-      <c r="O8" s="12">
+      <c r="N8" s="7">
+        <v>0</v>
+      </c>
+      <c r="O8" s="11">
         <v>0</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
-      <c r="Q8" s="8">
-        <v>0</v>
-      </c>
-      <c r="R8" s="12">
+      <c r="Q8" s="7">
+        <v>0</v>
+      </c>
+      <c r="R8" s="11">
         <v>0</v>
       </c>
       <c r="S8">
         <v>0</v>
       </c>
-      <c r="T8" s="8">
-        <v>0</v>
-      </c>
-      <c r="U8" s="12">
+      <c r="T8" s="7">
+        <v>0</v>
+      </c>
+      <c r="U8" s="11">
         <v>0</v>
       </c>
       <c r="V8">
         <v>0</v>
       </c>
-      <c r="W8" s="8">
+      <c r="W8" s="7">
         <v>0</v>
       </c>
       <c r="X8">
@@ -1065,74 +1078,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:26">
       <c r="A9" s="2">
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" s="8">
-        <v>0</v>
-      </c>
-      <c r="F9" s="12">
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
         <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9" s="8">
-        <v>0</v>
-      </c>
-      <c r="I9" s="12">
+      <c r="H9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11">
         <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
-      <c r="K9" s="8">
-        <v>0</v>
-      </c>
-      <c r="L9" s="12">
+      <c r="K9" s="7">
+        <v>0</v>
+      </c>
+      <c r="L9" s="11">
         <v>0</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
-      <c r="N9" s="8">
-        <v>0</v>
-      </c>
-      <c r="O9" s="12">
+      <c r="N9" s="7">
+        <v>0</v>
+      </c>
+      <c r="O9" s="11">
         <v>0</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
-      <c r="Q9" s="8">
-        <v>0</v>
-      </c>
-      <c r="R9" s="12">
+      <c r="Q9" s="7">
+        <v>0</v>
+      </c>
+      <c r="R9" s="11">
         <v>0</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
-      <c r="T9" s="8">
-        <v>0</v>
-      </c>
-      <c r="U9" s="12">
+      <c r="T9" s="7">
+        <v>0</v>
+      </c>
+      <c r="U9" s="11">
         <v>0</v>
       </c>
       <c r="V9">
         <v>0</v>
       </c>
-      <c r="W9" s="8">
+      <c r="W9" s="7">
         <v>0</v>
       </c>
       <c r="X9">
@@ -1140,74 +1153,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:26">
       <c r="A10" s="2">
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" s="8">
-        <v>0</v>
-      </c>
-      <c r="F10" s="12">
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="11">
         <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" s="8">
-        <v>0</v>
-      </c>
-      <c r="I10" s="12">
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
         <v>0</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10" s="8">
-        <v>0</v>
-      </c>
-      <c r="L10" s="12">
+      <c r="K10" s="7">
+        <v>0</v>
+      </c>
+      <c r="L10" s="11">
         <v>0</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="N10" s="8">
-        <v>0</v>
-      </c>
-      <c r="O10" s="12">
+      <c r="N10" s="7">
+        <v>0</v>
+      </c>
+      <c r="O10" s="11">
         <v>0</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
-      <c r="Q10" s="8">
-        <v>0</v>
-      </c>
-      <c r="R10" s="12">
+      <c r="Q10" s="7">
+        <v>0</v>
+      </c>
+      <c r="R10" s="11">
         <v>0</v>
       </c>
       <c r="S10">
         <v>0</v>
       </c>
-      <c r="T10" s="8">
-        <v>0</v>
-      </c>
-      <c r="U10" s="12">
+      <c r="T10" s="7">
+        <v>0</v>
+      </c>
+      <c r="U10" s="11">
         <v>0</v>
       </c>
       <c r="V10">
         <v>0</v>
       </c>
-      <c r="W10" s="8">
+      <c r="W10" s="7">
         <v>0</v>
       </c>
       <c r="X10">
@@ -1215,74 +1228,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:26">
       <c r="A11" s="2">
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>0</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
-      <c r="F11" s="12">
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="11">
         <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11" s="8">
-        <v>0</v>
-      </c>
-      <c r="I11" s="12">
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="11">
         <v>0</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
-      <c r="K11" s="8">
-        <v>0</v>
-      </c>
-      <c r="L11" s="12">
+      <c r="K11" s="7">
+        <v>0</v>
+      </c>
+      <c r="L11" s="11">
         <v>0</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
-      <c r="N11" s="8">
-        <v>0</v>
-      </c>
-      <c r="O11" s="12">
+      <c r="N11" s="7">
+        <v>0</v>
+      </c>
+      <c r="O11" s="11">
         <v>0</v>
       </c>
       <c r="P11">
         <v>0</v>
       </c>
-      <c r="Q11" s="8">
-        <v>0</v>
-      </c>
-      <c r="R11" s="12">
+      <c r="Q11" s="7">
+        <v>0</v>
+      </c>
+      <c r="R11" s="11">
         <v>0</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
-      <c r="T11" s="8">
-        <v>0</v>
-      </c>
-      <c r="U11" s="12">
+      <c r="T11" s="7">
+        <v>0</v>
+      </c>
+      <c r="U11" s="11">
         <v>0</v>
       </c>
       <c r="V11">
         <v>0</v>
       </c>
-      <c r="W11" s="8">
+      <c r="W11" s="7">
         <v>0</v>
       </c>
       <c r="X11">
@@ -1290,74 +1303,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:26">
       <c r="A12" s="2">
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" s="8">
-        <v>0</v>
-      </c>
-      <c r="F12" s="12">
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11">
         <v>0</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12" s="8">
-        <v>0</v>
-      </c>
-      <c r="I12" s="12">
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="11">
         <v>0</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
-      <c r="K12" s="8">
-        <v>0</v>
-      </c>
-      <c r="L12" s="12">
+      <c r="K12" s="7">
+        <v>0</v>
+      </c>
+      <c r="L12" s="11">
         <v>0</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
-      <c r="N12" s="8">
-        <v>0</v>
-      </c>
-      <c r="O12" s="12">
+      <c r="N12" s="7">
+        <v>0</v>
+      </c>
+      <c r="O12" s="11">
         <v>0</v>
       </c>
       <c r="P12">
         <v>0</v>
       </c>
-      <c r="Q12" s="8">
-        <v>0</v>
-      </c>
-      <c r="R12" s="12">
+      <c r="Q12" s="7">
+        <v>0</v>
+      </c>
+      <c r="R12" s="11">
         <v>0</v>
       </c>
       <c r="S12">
         <v>0</v>
       </c>
-      <c r="T12" s="8">
-        <v>0</v>
-      </c>
-      <c r="U12" s="12">
+      <c r="T12" s="7">
+        <v>0</v>
+      </c>
+      <c r="U12" s="11">
         <v>0</v>
       </c>
       <c r="V12">
         <v>0</v>
       </c>
-      <c r="W12" s="8">
+      <c r="W12" s="7">
         <v>0</v>
       </c>
       <c r="X12">
@@ -1365,74 +1378,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:26">
       <c r="A13" s="2">
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <v>0</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" s="8">
-        <v>0</v>
-      </c>
-      <c r="F13" s="12">
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11">
         <v>0</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13" s="8">
-        <v>0</v>
-      </c>
-      <c r="I13" s="12">
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
         <v>0</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
-      <c r="K13" s="8">
-        <v>0</v>
-      </c>
-      <c r="L13" s="12">
+      <c r="K13" s="7">
+        <v>0</v>
+      </c>
+      <c r="L13" s="11">
         <v>0</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
-      <c r="N13" s="8">
-        <v>0</v>
-      </c>
-      <c r="O13" s="12">
+      <c r="N13" s="7">
+        <v>0</v>
+      </c>
+      <c r="O13" s="11">
         <v>0</v>
       </c>
       <c r="P13">
         <v>0</v>
       </c>
-      <c r="Q13" s="8">
-        <v>0</v>
-      </c>
-      <c r="R13" s="12">
+      <c r="Q13" s="7">
+        <v>0</v>
+      </c>
+      <c r="R13" s="11">
         <v>0</v>
       </c>
       <c r="S13">
         <v>0</v>
       </c>
-      <c r="T13" s="8">
-        <v>0</v>
-      </c>
-      <c r="U13" s="12">
+      <c r="T13" s="7">
+        <v>0</v>
+      </c>
+      <c r="U13" s="11">
         <v>0</v>
       </c>
       <c r="V13">
         <v>0</v>
       </c>
-      <c r="W13" s="8">
+      <c r="W13" s="7">
         <v>0</v>
       </c>
       <c r="X13">
@@ -1440,74 +1453,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:26">
       <c r="A14" s="2">
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <v>0</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" s="8">
-        <v>0</v>
-      </c>
-      <c r="F14" s="12">
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11">
         <v>0</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14" s="8">
-        <v>0</v>
-      </c>
-      <c r="I14" s="12">
+      <c r="H14" s="7">
+        <v>0</v>
+      </c>
+      <c r="I14" s="11">
         <v>0</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
-      <c r="K14" s="8">
-        <v>0</v>
-      </c>
-      <c r="L14" s="12">
+      <c r="K14" s="7">
+        <v>0</v>
+      </c>
+      <c r="L14" s="11">
         <v>0</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
-      <c r="N14" s="8">
-        <v>0</v>
-      </c>
-      <c r="O14" s="12">
+      <c r="N14" s="7">
+        <v>0</v>
+      </c>
+      <c r="O14" s="11">
         <v>0</v>
       </c>
       <c r="P14">
         <v>0</v>
       </c>
-      <c r="Q14" s="8">
-        <v>0</v>
-      </c>
-      <c r="R14" s="12">
+      <c r="Q14" s="7">
+        <v>0</v>
+      </c>
+      <c r="R14" s="11">
         <v>0</v>
       </c>
       <c r="S14">
         <v>0</v>
       </c>
-      <c r="T14" s="8">
-        <v>0</v>
-      </c>
-      <c r="U14" s="12">
+      <c r="T14" s="7">
+        <v>0</v>
+      </c>
+      <c r="U14" s="11">
         <v>0</v>
       </c>
       <c r="V14">
         <v>0</v>
       </c>
-      <c r="W14" s="8">
+      <c r="W14" s="7">
         <v>0</v>
       </c>
       <c r="X14">
@@ -1515,74 +1528,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:26">
       <c r="A15" s="2">
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15" s="8">
-        <v>0</v>
-      </c>
-      <c r="F15" s="12">
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
         <v>0</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
-      <c r="H15" s="8">
-        <v>0</v>
-      </c>
-      <c r="I15" s="12">
+      <c r="H15" s="7">
+        <v>0</v>
+      </c>
+      <c r="I15" s="11">
         <v>0</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
-      <c r="K15" s="8">
-        <v>0</v>
-      </c>
-      <c r="L15" s="12">
+      <c r="K15" s="7">
+        <v>0</v>
+      </c>
+      <c r="L15" s="11">
         <v>0</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
-      <c r="N15" s="8">
-        <v>0</v>
-      </c>
-      <c r="O15" s="12">
+      <c r="N15" s="7">
+        <v>0</v>
+      </c>
+      <c r="O15" s="11">
         <v>0</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
-      <c r="Q15" s="8">
-        <v>0</v>
-      </c>
-      <c r="R15" s="12">
+      <c r="Q15" s="7">
+        <v>0</v>
+      </c>
+      <c r="R15" s="11">
         <v>0</v>
       </c>
       <c r="S15">
         <v>0</v>
       </c>
-      <c r="T15" s="8">
-        <v>0</v>
-      </c>
-      <c r="U15" s="12">
+      <c r="T15" s="7">
+        <v>0</v>
+      </c>
+      <c r="U15" s="11">
         <v>0</v>
       </c>
       <c r="V15">
         <v>0</v>
       </c>
-      <c r="W15" s="8">
+      <c r="W15" s="7">
         <v>0</v>
       </c>
       <c r="X15">
@@ -1590,74 +1603,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:26">
       <c r="A16" s="2">
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <v>0</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16" s="8">
-        <v>0</v>
-      </c>
-      <c r="F16" s="12">
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="11">
         <v>0</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
-      <c r="H16" s="8">
-        <v>0</v>
-      </c>
-      <c r="I16" s="12">
+      <c r="H16" s="7">
+        <v>0</v>
+      </c>
+      <c r="I16" s="11">
         <v>0</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
-      <c r="K16" s="8">
-        <v>0</v>
-      </c>
-      <c r="L16" s="12">
+      <c r="K16" s="7">
+        <v>0</v>
+      </c>
+      <c r="L16" s="11">
         <v>0</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
-      <c r="N16" s="8">
-        <v>0</v>
-      </c>
-      <c r="O16" s="12">
+      <c r="N16" s="7">
+        <v>0</v>
+      </c>
+      <c r="O16" s="11">
         <v>0</v>
       </c>
       <c r="P16">
         <v>0</v>
       </c>
-      <c r="Q16" s="8">
-        <v>0</v>
-      </c>
-      <c r="R16" s="12">
+      <c r="Q16" s="7">
+        <v>0</v>
+      </c>
+      <c r="R16" s="11">
         <v>0</v>
       </c>
       <c r="S16">
         <v>0</v>
       </c>
-      <c r="T16" s="8">
-        <v>0</v>
-      </c>
-      <c r="U16" s="12">
+      <c r="T16" s="7">
+        <v>0</v>
+      </c>
+      <c r="U16" s="11">
         <v>0</v>
       </c>
       <c r="V16">
         <v>0</v>
       </c>
-      <c r="W16" s="8">
+      <c r="W16" s="7">
         <v>0</v>
       </c>
       <c r="X16">
@@ -1672,67 +1685,67 @@
       <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>0</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
-      <c r="E17" s="8">
-        <v>0</v>
-      </c>
-      <c r="F17" s="12">
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11">
         <v>0</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
-      <c r="H17" s="8">
-        <v>0</v>
-      </c>
-      <c r="I17" s="12">
+      <c r="H17" s="7">
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
         <v>0</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
-      <c r="K17" s="8">
-        <v>0</v>
-      </c>
-      <c r="L17" s="12">
+      <c r="K17" s="7">
+        <v>0</v>
+      </c>
+      <c r="L17" s="11">
         <v>0</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
-      <c r="N17" s="8">
-        <v>0</v>
-      </c>
-      <c r="O17" s="12">
+      <c r="N17" s="7">
+        <v>0</v>
+      </c>
+      <c r="O17" s="11">
         <v>0</v>
       </c>
       <c r="P17">
         <v>0</v>
       </c>
-      <c r="Q17" s="8">
-        <v>0</v>
-      </c>
-      <c r="R17" s="12">
+      <c r="Q17" s="7">
+        <v>0</v>
+      </c>
+      <c r="R17" s="11">
         <v>0</v>
       </c>
       <c r="S17">
         <v>0</v>
       </c>
-      <c r="T17" s="8">
-        <v>0</v>
-      </c>
-      <c r="U17" s="12">
+      <c r="T17" s="7">
+        <v>0</v>
+      </c>
+      <c r="U17" s="11">
         <v>0</v>
       </c>
       <c r="V17">
         <v>0</v>
       </c>
-      <c r="W17" s="8">
+      <c r="W17" s="7">
         <v>0</v>
       </c>
       <c r="X17">
@@ -1747,67 +1760,67 @@
       <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <v>0</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18" s="8">
-        <v>0</v>
-      </c>
-      <c r="F18" s="12">
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11">
         <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
-      <c r="H18" s="8">
-        <v>0</v>
-      </c>
-      <c r="I18" s="12">
+      <c r="H18" s="7">
+        <v>0</v>
+      </c>
+      <c r="I18" s="11">
         <v>0</v>
       </c>
       <c r="J18">
         <v>0</v>
       </c>
-      <c r="K18" s="8">
-        <v>0</v>
-      </c>
-      <c r="L18" s="12">
+      <c r="K18" s="7">
+        <v>0</v>
+      </c>
+      <c r="L18" s="11">
         <v>0</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
-      <c r="N18" s="8">
-        <v>0</v>
-      </c>
-      <c r="O18" s="12">
+      <c r="N18" s="7">
+        <v>0</v>
+      </c>
+      <c r="O18" s="11">
         <v>0</v>
       </c>
       <c r="P18">
         <v>0</v>
       </c>
-      <c r="Q18" s="8">
-        <v>0</v>
-      </c>
-      <c r="R18" s="12">
+      <c r="Q18" s="7">
+        <v>0</v>
+      </c>
+      <c r="R18" s="11">
         <v>0</v>
       </c>
       <c r="S18">
         <v>0</v>
       </c>
-      <c r="T18" s="8">
-        <v>0</v>
-      </c>
-      <c r="U18" s="12">
+      <c r="T18" s="7">
+        <v>0</v>
+      </c>
+      <c r="U18" s="11">
         <v>0</v>
       </c>
       <c r="V18">
         <v>0</v>
       </c>
-      <c r="W18" s="8">
+      <c r="W18" s="7">
         <v>0</v>
       </c>
       <c r="X18">
@@ -1822,67 +1835,67 @@
       <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-      <c r="F19" s="12">
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19" s="11">
         <v>0</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
-      <c r="H19" s="8">
-        <v>0</v>
-      </c>
-      <c r="I19" s="12">
+      <c r="H19" s="7">
+        <v>0</v>
+      </c>
+      <c r="I19" s="11">
         <v>0</v>
       </c>
       <c r="J19">
         <v>0</v>
       </c>
-      <c r="K19" s="8">
-        <v>0</v>
-      </c>
-      <c r="L19" s="12">
+      <c r="K19" s="7">
+        <v>0</v>
+      </c>
+      <c r="L19" s="11">
         <v>0</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
-      <c r="N19" s="8">
-        <v>0</v>
-      </c>
-      <c r="O19" s="12">
+      <c r="N19" s="7">
+        <v>0</v>
+      </c>
+      <c r="O19" s="11">
         <v>0</v>
       </c>
       <c r="P19">
         <v>0</v>
       </c>
-      <c r="Q19" s="8">
-        <v>0</v>
-      </c>
-      <c r="R19" s="12">
+      <c r="Q19" s="7">
+        <v>0</v>
+      </c>
+      <c r="R19" s="11">
         <v>0</v>
       </c>
       <c r="S19">
         <v>0</v>
       </c>
-      <c r="T19" s="8">
-        <v>0</v>
-      </c>
-      <c r="U19" s="12">
+      <c r="T19" s="7">
+        <v>0</v>
+      </c>
+      <c r="U19" s="11">
         <v>0</v>
       </c>
       <c r="V19">
         <v>0</v>
       </c>
-      <c r="W19" s="8">
+      <c r="W19" s="7">
         <v>0</v>
       </c>
       <c r="X19">
@@ -1897,67 +1910,67 @@
       <c r="B20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="11">
         <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20" s="8">
-        <v>0</v>
-      </c>
-      <c r="F20" s="12">
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
         <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
-      <c r="H20" s="8">
-        <v>0</v>
-      </c>
-      <c r="I20" s="12">
+      <c r="H20" s="7">
+        <v>0</v>
+      </c>
+      <c r="I20" s="11">
         <v>0</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
-      <c r="K20" s="8">
-        <v>0</v>
-      </c>
-      <c r="L20" s="12">
+      <c r="K20" s="7">
+        <v>0</v>
+      </c>
+      <c r="L20" s="11">
         <v>0</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
-      <c r="N20" s="8">
-        <v>0</v>
-      </c>
-      <c r="O20" s="12">
+      <c r="N20" s="7">
+        <v>0</v>
+      </c>
+      <c r="O20" s="11">
         <v>0</v>
       </c>
       <c r="P20">
         <v>0</v>
       </c>
-      <c r="Q20" s="8">
-        <v>0</v>
-      </c>
-      <c r="R20" s="12">
+      <c r="Q20" s="7">
+        <v>0</v>
+      </c>
+      <c r="R20" s="11">
         <v>0</v>
       </c>
       <c r="S20">
         <v>0</v>
       </c>
-      <c r="T20" s="8">
-        <v>0</v>
-      </c>
-      <c r="U20" s="12">
+      <c r="T20" s="7">
+        <v>0</v>
+      </c>
+      <c r="U20" s="11">
         <v>0</v>
       </c>
       <c r="V20">
         <v>0</v>
       </c>
-      <c r="W20" s="8">
+      <c r="W20" s="7">
         <v>0</v>
       </c>
       <c r="X20">

</xml_diff>